<commit_message>
added PMID and notes columns to data structure
</commit_message>
<xml_diff>
--- a/R_ignore/example_data.xlsx
+++ b/R_ignore/example_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rverity/Dropbox/Bob/Work/My Programs/Mapping/STAVE/R_ignore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E28833-F568-5749-B411-F1F1C48AFA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7907A17-5759-EB45-BB34-66795B3B93AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3720" windowWidth="28040" windowHeight="17180" activeTab="2" xr2:uid="{5E2F86C7-B2CE-7148-AC3A-7062C99AC2A0}"/>
+    <workbookView xWindow="3840" yWindow="3360" windowWidth="28040" windowHeight="17180" activeTab="2" xr2:uid="{5E2F86C7-B2CE-7148-AC3A-7062C99AC2A0}"/>
   </bookViews>
   <sheets>
     <sheet name="studies" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
   <si>
     <t>study_id</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>Asua_2019_Mubende_2017</t>
+  </si>
+  <si>
+    <t>PMID</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -1050,15 +1056,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B9AA3ED-F91D-AA46-B405-7D23BD7454F3}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1080,8 +1086,11 @@
       <c r="G1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1101,7 +1110,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1398,15 +1407,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F3FAB6-1D43-BA44-B480-93F0FE148201}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1422,8 +1431,11 @@
       <c r="E1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1440,7 +1452,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1457,7 +1469,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1474,7 +1486,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1491,7 +1503,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1508,7 +1520,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1525,7 +1537,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1542,7 +1554,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1559,7 +1571,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1576,7 +1588,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>

</xml_diff>